<commit_message>
Converted reward values (.xlsx/.csv) to integer values. Structs now read in rewards as string and then convert to Int to resolve string to float conversion issues
</commit_message>
<xml_diff>
--- a/HungerRewards.xlsx
+++ b/HungerRewards.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451CE800-7CA7-4540-B843-5871BC3A90BE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2309FE-E5DC-4220-B673-5346D6E7CC0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,10 +423,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-0.5</v>
+        <v>-10</v>
       </c>
       <c r="D2">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -437,10 +437,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-0.5</v>
+        <v>-10</v>
       </c>
       <c r="D3">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -451,10 +451,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>-0.5</v>
+        <v>-10</v>
       </c>
       <c r="D4">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -465,10 +465,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>-0.5</v>
+        <v>-10</v>
       </c>
       <c r="D5">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-0.5</v>
+        <v>-10</v>
       </c>
       <c r="D6">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,13 +490,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,13 +504,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,13 +518,13 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,13 +532,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,13 +546,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,13 +560,13 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0.99</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,13 +574,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.99</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,13 +588,13 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.99</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,13 +602,13 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.99</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>0.99</v>
+        <v>20</v>
       </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>-0.99</v>
+        <v>-20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed negative rewards values, Updated data tables with new values
</commit_message>
<xml_diff>
--- a/HungerRewards.xlsx
+++ b/HungerRewards.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2309FE-E5DC-4220-B673-5346D6E7CC0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DAE6F9-E3BB-45B1-A9F9-D9B680B0B3E2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>LOW</t>
   </si>
@@ -75,6 +74,9 @@
   </si>
   <si>
     <t>HIGHFLEE</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -395,7 +397,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,11 +424,11 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>-10</v>
-      </c>
-      <c r="D2">
-        <v>-20</v>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -436,11 +438,11 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>-10</v>
-      </c>
-      <c r="D3">
-        <v>-20</v>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,11 +452,11 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>-10</v>
-      </c>
-      <c r="D4">
-        <v>-20</v>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,11 +466,11 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>-10</v>
-      </c>
-      <c r="D5">
-        <v>-20</v>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,11 +480,11 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>-10</v>
-      </c>
-      <c r="D6">
-        <v>-20</v>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -495,8 +497,8 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7">
-        <v>-20</v>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,8 +511,8 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8">
-        <v>-20</v>
+      <c r="D8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,8 +525,8 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9">
-        <v>-20</v>
+      <c r="D9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -537,8 +539,8 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>-20</v>
+      <c r="D10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -551,8 +553,8 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>-20</v>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -565,8 +567,8 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12">
-        <v>-20</v>
+      <c r="D12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,8 +581,8 @@
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13">
-        <v>-20</v>
+      <c r="D13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -593,8 +595,8 @@
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14">
-        <v>-20</v>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,8 +609,8 @@
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15">
-        <v>-20</v>
+      <c r="D15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,23 +623,11 @@
       <c r="C16">
         <v>10</v>
       </c>
-      <c r="D16">
-        <v>-20</v>
+      <c r="D16" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D7FC2A-1159-4EB7-8DC0-259ED1094762}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>